<commit_message>
86555-Added aspose license, unit tests and some more chart changes.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/ILRProvidersReturningFirstTimePerDayTemplate.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/ILRProvidersReturningFirstTimePerDayTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719F3528-B6B2-4D26-A1D0-C962627B473D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311AF68A-5365-4DAF-99AB-E5719A6282D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5F8E5E8B-81CE-49AB-8EE1-D1C01E6C85E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5F8E5E8B-81CE-49AB-8EE1-D1C01E6C85E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart - ILR No of Provider Ret" sheetId="2" r:id="rId1"/>
@@ -186,6 +186,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCC66"/>
       <color rgb="FFFF9933"/>
     </mruColors>
   </colors>
@@ -217,7 +218,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>'Chart - ILR No of Provider Ret'!$V$36</c:f>
+          <c:f>'Chart - ILR No of Provider Ret'!$V$31</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -239,7 +240,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -288,7 +289,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="FFCC66"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -302,7 +303,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FFCC66"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -321,7 +322,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FFCC66"/>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
@@ -397,18 +398,18 @@
             <c:strRef>
               <c:f>'Chart - ILR No of Provider Ret'!$C$35:$C$71</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>&amp;=IlrReturningProvidersInfo.IlrProvidersReturningFirstTimePerDaysList.DaysToClose</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-25</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>-29</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
+                <c:pt idx="3">
+                  <c:v>-28</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -426,9 +427,9 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -448,7 +449,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="35"/>
+        <c:gapWidth val="25"/>
         <c:overlap val="-27"/>
         <c:axId val="668370608"/>
         <c:axId val="668372576"/>
@@ -467,7 +468,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -480,7 +481,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Days Before Period Close</a:t>
                 </a:r>
               </a:p>
@@ -507,7 +508,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -544,7 +545,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -595,7 +596,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -608,22 +609,22 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" b="1"/>
                   <a:t>No. of</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:rPr lang="en-GB" b="1" baseline="0"/>
                   <a:t> 1st </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" b="1"/>
                   <a:t> time submitting providers (Log 2 scalre)</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:rPr lang="en-GB" b="1" baseline="0"/>
                   <a:t> </a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB"/>
+                <a:endParaRPr lang="en-GB" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -640,7 +641,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -676,7 +677,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1286,15 +1287,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23811</xdr:colOff>
+      <xdr:colOff>23810</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>152398</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1621,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F817F05-25C8-49E4-8BFD-D49A1B0DB880}">
   <dimension ref="C26:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,37 +1631,41 @@
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="21" max="22" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="26" spans="3:18" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:22" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="3:18" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="V31" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="3:22" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C32" s="8" t="s">
         <v>4</v>
       </c>
@@ -1680,11 +1685,11 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
     </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="3:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:6" ht="21" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="3:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>3</v>
       </c>
@@ -1700,70 +1705,67 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="3:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="3">
-        <v>-25</v>
+        <v>-30</v>
       </c>
       <c r="D36" s="4">
         <v>2</v>
       </c>
-      <c r="V36" s="2" t="s">
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="3">
+        <v>-29</v>
+      </c>
+      <c r="D37" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="3">
+        <v>-28</v>
+      </c>
+      <c r="D38" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C37" s="3">
-        <v>10</v>
-      </c>
-      <c r="D37" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="3">
-        <v>5</v>
-      </c>
-      <c r="D39" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="3"/>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" s="3"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" s="3"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C47" s="3"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" s="3"/>
       <c r="D48" s="4"/>
     </row>

</xml_diff>

<commit_message>
86555 - Another round of Template changes, unit tests and refactoring.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.Operations.Reports.Reports/Templates/ILRProvidersReturningFirstTimePerDayTemplate.xlsx
+++ b/src/ESFA.DC.Operations.Reports.Reports/Templates/ILRProvidersReturningFirstTimePerDayTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSTS\DCT\DC-Operations-Reports\src\ESFA.DC.Operations.Reports.Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311AF68A-5365-4DAF-99AB-E5719A6282D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79AB03F-47CC-4941-A58E-178AA1F500F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5F8E5E8B-81CE-49AB-8EE1-D1C01E6C85E9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5F8E5E8B-81CE-49AB-8EE1-D1C01E6C85E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart - ILR No of Provider Ret" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <numFmt numFmtId="164" formatCode="[$-10809]#,##0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]#,##0;\-#,##0;&quot;-&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +105,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF8B0000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -153,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -178,6 +185,9 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,18 +408,9 @@
             <c:strRef>
               <c:f>'Chart - ILR No of Provider Ret'!$C$35:$C$71</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>&amp;=IlrReturningProvidersInfo.IlrProvidersReturningFirstTimePerDaysList.DaysToClose</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-29</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-28</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -422,15 +423,6 @@
                 <c:ptCount val="37"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1623,7 +1615,7 @@
   <dimension ref="C26:V92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:D38"/>
+      <selection activeCell="C32" sqref="C32:R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,24 +1658,24 @@
       </c>
     </row>
     <row r="32" spans="3:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
@@ -1706,28 +1698,16 @@
       </c>
     </row>
     <row r="36" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="3">
-        <v>-30</v>
-      </c>
-      <c r="D36" s="4">
-        <v>2</v>
-      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="3">
-        <v>-29</v>
-      </c>
-      <c r="D37" s="4">
-        <v>4</v>
-      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="3">
-        <v>-28</v>
-      </c>
-      <c r="D38" s="4">
-        <v>5</v>
-      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>

</xml_diff>